<commit_message>
added 2 collumns with extra info
</commit_message>
<xml_diff>
--- a/data/standards_mzml.xlsx
+++ b/data/standards_mzml.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t xml:space="preserve">mzML</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">sample_name</t>
   </si>
   <si>
+    <t xml:space="preserve">sample_origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC_LowIS_Mix13_1_POS.mzML</t>
   </si>
   <si>
@@ -59,6 +65,12 @@
   </si>
   <si>
     <t xml:space="preserve">low_a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pool QC</t>
   </si>
   <si>
     <t xml:space="preserve">QC_HighIS_Mix13_3_POS.mzML</t>
@@ -211,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,6 +234,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -416,18 +440,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -453,415 +478,227 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
+      <c r="I8" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="G10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="G11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="G12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="G13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="G14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="G15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="G16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="G17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="G18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="G19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="G20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="G21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="G22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="E23" s="0"/>
-      <c r="G23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="G24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="E25" s="0"/>
-      <c r="G25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="E26" s="0"/>
-      <c r="G26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="E27" s="0"/>
-      <c r="G27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="G28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="G29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="C30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="G30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="G31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="G32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="C33" s="0"/>
-      <c r="E33" s="0"/>
-      <c r="G33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="C34" s="0"/>
-      <c r="E34" s="0"/>
-      <c r="G34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="C35" s="0"/>
-      <c r="E35" s="0"/>
-      <c r="G35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="C36" s="0"/>
-      <c r="E36" s="0"/>
-      <c r="G36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="C37" s="0"/>
-      <c r="E37" s="0"/>
-      <c r="G37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="E38" s="0"/>
-      <c r="G38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="E39" s="0"/>
-      <c r="G39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="G40" s="0"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="G41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="C42" s="0"/>
-      <c r="E42" s="0"/>
-      <c r="G42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="C43" s="0"/>
-      <c r="E43" s="0"/>
-      <c r="G43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="E44" s="0"/>
-      <c r="G44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="C45" s="0"/>
-      <c r="E45" s="0"/>
-      <c r="G45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="E46" s="0"/>
-      <c r="G46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0"/>
-      <c r="C47" s="0"/>
-      <c r="E47" s="0"/>
-      <c r="G47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0"/>
-      <c r="C48" s="0"/>
-      <c r="E48" s="0"/>
-      <c r="G48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0"/>
-      <c r="C49" s="0"/>
-      <c r="E49" s="0"/>
-      <c r="G49" s="0"/>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>